<commit_message>
act plantilla cubicaje 4
</commit_message>
<xml_diff>
--- a/public/img/cubicaje/plantilla/Plantilla_cubicaje.xlsx
+++ b/public/img/cubicaje/plantilla/Plantilla_cubicaje.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proyectos\forespama\public\img\cubicaje\plantilla\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{948AC776-733D-4D79-851B-BAD7603AC58D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11F24697-7DC0-4803-BEBC-06FE2DFDAAE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7E53B437-93E4-489B-B999-F997A8209410}"/>
   </bookViews>
@@ -517,8 +517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD801732-F107-4B6C-B4DB-E5A05BA38E87}">
   <dimension ref="A1:D200"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
+      <selection activeCell="C200" sqref="C200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1935,6 +1935,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="VWuBg8ns6Jj6HBQ4mGdR3AoNETsbDxUTUlK/eR5cxezsZjrU7RSkxDFPHoVKp7lDKOX4Pd168EWo+trueAjLeg==" saltValue="HR+H6Fh0yjwEvRVCwpAHpg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <dataValidations count="1">
     <dataValidation type="textLength" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{105A2C15-C371-47DE-810D-D9A31233B48E}">
       <formula1>11</formula1>

</xml_diff>